<commit_message>
Solutions till 5-59 added. Starting 5-60...
</commit_message>
<xml_diff>
--- a/Chapter 5/5-56.xlsx
+++ b/Chapter 5/5-56.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\OneDrive\Desktop\Introduction to Financial Accounting\Chapter 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DEECF4A-645D-4B82-B23B-76509F9B27B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EFDA1B-D28E-4EED-B989-65A757872178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{50587594-6B36-48F8-BC48-11534DCBD882}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Statement of Cash Flow" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,10 +35,101 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>Particulars</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Name : Jacinta Manufacturing Co. (JMC)</t>
+  </si>
+  <si>
+    <t>Cash flow by Operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Cash Sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Received from Outstanding A/c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Operation Expenses:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Purchase of goods on cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Salaries expense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Other Operational expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Income Tax Applied</t>
+  </si>
+  <si>
+    <t>Total from Operations</t>
+  </si>
+  <si>
+    <t>Cash flow by Investments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Purchase of welding machines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Sales of old stock</t>
+  </si>
+  <si>
+    <t>Total from Investments</t>
+  </si>
+  <si>
+    <t>Cash flow from Finance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Issued a Long Term Debt</t>
+  </si>
+  <si>
+    <t>Total from Finance</t>
+  </si>
+  <si>
+    <t>Net cash flow from activities</t>
+  </si>
+  <si>
+    <t>Cash &amp; Cash Equivalents on 31 Dec, 2010</t>
+  </si>
+  <si>
+    <t>Cash &amp; Cash Equivalents on 31 Dec, 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Total Operational Expenses </t>
+  </si>
+  <si>
+    <t>STATEMENT OF CASH FLOW AS OF 31 DEC, 2011 (in thousands of $)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -66,8 +157,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +501,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBB0F32-9DEE-4217-8E30-0BB14746B4C2}">
-  <dimension ref="A1"/>
+  <dimension ref="I5:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="9" max="9" width="25.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="11" max="11" width="2.109375" customWidth="1"/>
+    <col min="12" max="12" width="2.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="K5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="M7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="12" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="15" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M15">
+        <v>-82</v>
+      </c>
+    </row>
+    <row r="16" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="17" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17">
+        <f>SUM(M14:M16)</f>
+        <v>-397</v>
+      </c>
+    </row>
+    <row r="18" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="20" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" s="1">
+        <f>SUM(N11:N18)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23">
+        <v>-125</v>
+      </c>
+    </row>
+    <row r="24" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="1">
+        <f>SUM(M23:M24)</f>
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="28" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I28" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I29" t="s">
+        <v>19</v>
+      </c>
+      <c r="M29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N31" s="1">
+        <f>SUM(M29)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N33" s="1">
+        <f>SUM(N20, N26, N31)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I34" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="9:14" x14ac:dyDescent="0.3">
+      <c r="I36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N36" s="1">
+        <f>SUM(N33:N34)</f>
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M7:N7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>